<commit_message>
add fcn() for None at reindexPOSCAR_v2.ipynb
</commit_message>
<xml_diff>
--- a/06_distance_LitoLi_intercage_litype4_CONTCAR_positive_0.xlsx
+++ b/06_distance_LitoLi_intercage_litype4_CONTCAR_positive_0.xlsx
@@ -472,28 +472,28 @@
         <v>0</v>
       </c>
       <c r="C2" t="n">
-        <v>0.1599042420245013</v>
+        <v>0.002767164346438711</v>
       </c>
       <c r="D2" t="n">
-        <v>0.4873425835964197</v>
+        <v>0.005534328692877489</v>
       </c>
       <c r="E2" t="n">
-        <v>0.3889554917784543</v>
+        <v>0.002767164346438755</v>
       </c>
       <c r="F2" t="n">
-        <v>0.02478433142909525</v>
+        <v>0.008301493039316252</v>
       </c>
       <c r="G2" t="n">
-        <v>0.435567315948924</v>
+        <v>0.005534328692877542</v>
       </c>
       <c r="H2" t="n">
-        <v>0.488464116688748</v>
+        <v>0.008301493039316252</v>
       </c>
       <c r="I2" t="n">
-        <v>0.3713553935490552</v>
+        <v>0.0166029860786326</v>
       </c>
       <c r="J2" t="n">
-        <v>0.4652969783925895</v>
+        <v>0.0110686573857551</v>
       </c>
     </row>
     <row r="3">
@@ -506,28 +506,28 @@
         <v>0</v>
       </c>
       <c r="C3" t="n">
-        <v>0.03345822752206347</v>
+        <v>0.001396708916112762</v>
       </c>
       <c r="D3" t="n">
-        <v>0.3420095787884608</v>
+        <v>0.0027934178322257</v>
       </c>
       <c r="E3" t="n">
-        <v>0.6135651015221841</v>
+        <v>0.001396708916112888</v>
       </c>
       <c r="F3" t="n">
-        <v>0.2941927463953483</v>
+        <v>0.004190126748338587</v>
       </c>
       <c r="G3" t="n">
-        <v>0.3198602685326024</v>
+        <v>0.002793417832225825</v>
       </c>
       <c r="H3" t="n">
-        <v>0.3861190084316656</v>
+        <v>0.004190126748338714</v>
       </c>
       <c r="I3" t="n">
-        <v>0.6094891054902846</v>
+        <v>0.008380253496677301</v>
       </c>
       <c r="J3" t="n">
-        <v>0.7170912174806251</v>
+        <v>0.005586835664451475</v>
       </c>
     </row>
     <row r="4">
@@ -540,28 +540,28 @@
         <v>0</v>
       </c>
       <c r="C4" t="n">
-        <v>0.02331629159554082</v>
+        <v>0.01709710209335594</v>
       </c>
       <c r="D4" t="n">
-        <v>0.0239595163594701</v>
+        <v>0.03419420418671198</v>
       </c>
       <c r="E4" t="n">
-        <v>0.5329357336950329</v>
+        <v>0.01709710209335608</v>
       </c>
       <c r="F4" t="n">
-        <v>0.1404180705845086</v>
+        <v>0.05129130628006797</v>
       </c>
       <c r="G4" t="n">
-        <v>0.3329963333582</v>
+        <v>0.0341942041867121</v>
       </c>
       <c r="H4" t="n">
-        <v>0.3105934570171596</v>
+        <v>0.05129130628006809</v>
       </c>
       <c r="I4" t="n">
-        <v>0.6233732104249997</v>
+        <v>0.1025826125601361</v>
       </c>
       <c r="J4" t="n">
-        <v>0.7877718906765283</v>
+        <v>0.06838840837342415</v>
       </c>
     </row>
     <row r="5">
@@ -574,28 +574,28 @@
         <v>0</v>
       </c>
       <c r="C5" t="n">
-        <v>0.08492603540593104</v>
+        <v>0.008776272009646518</v>
       </c>
       <c r="D5" t="n">
-        <v>0.3934881152244841</v>
+        <v>0.0175525440192929</v>
       </c>
       <c r="E5" t="n">
-        <v>0.5176193094491501</v>
+        <v>0.008776272009646428</v>
       </c>
       <c r="F5" t="n">
-        <v>0.2483276680389734</v>
+        <v>0.02632881602893943</v>
       </c>
       <c r="G5" t="n">
-        <v>0.4249491875633597</v>
+        <v>0.01755254401929289</v>
       </c>
       <c r="H5" t="n">
-        <v>0.4050866709828661</v>
+        <v>0.02632881602893932</v>
       </c>
       <c r="I5" t="n">
-        <v>0.5556072474745622</v>
+        <v>0.05265763205787874</v>
       </c>
       <c r="J5" t="n">
-        <v>0.6450257546336378</v>
+        <v>0.03510508803858584</v>
       </c>
     </row>
     <row r="6">
@@ -608,28 +608,28 @@
         <v>0</v>
       </c>
       <c r="C6" t="n">
-        <v>0.02331629159554218</v>
+        <v>0.0045608954098372</v>
       </c>
       <c r="D6" t="n">
-        <v>0.02395951635948744</v>
+        <v>0.009121790819674305</v>
       </c>
       <c r="E6" t="n">
-        <v>0.5329357336949913</v>
+        <v>0.004560895409837224</v>
       </c>
       <c r="F6" t="n">
-        <v>0.1404180705846018</v>
+        <v>0.0136826862295115</v>
       </c>
       <c r="G6" t="n">
-        <v>0.3329963333581463</v>
+        <v>0.009121790819674274</v>
       </c>
       <c r="H6" t="n">
-        <v>0.3105934570171546</v>
+        <v>0.01368268622951148</v>
       </c>
       <c r="I6" t="n">
-        <v>0.6233732104247923</v>
+        <v>0.027365372459023</v>
       </c>
       <c r="J6" t="n">
-        <v>0.7877718906760864</v>
+        <v>0.0182435816393487</v>
       </c>
     </row>
     <row r="7">
@@ -642,28 +642,28 @@
         <v>0</v>
       </c>
       <c r="C7" t="n">
-        <v>0.0334582275220587</v>
+        <v>0.004265792029994007</v>
       </c>
       <c r="D7" t="n">
-        <v>0.3420095787860275</v>
+        <v>0.008531584059987994</v>
       </c>
       <c r="E7" t="n">
-        <v>0.6135651015297139</v>
+        <v>0.004265792029993986</v>
       </c>
       <c r="F7" t="n">
-        <v>0.2941927463888354</v>
+        <v>0.01279737608998207</v>
       </c>
       <c r="G7" t="n">
-        <v>0.3198602685305655</v>
+        <v>0.008531584059988061</v>
       </c>
       <c r="H7" t="n">
-        <v>0.3861190084316057</v>
+        <v>0.01279737608998205</v>
       </c>
       <c r="I7" t="n">
-        <v>0.6094891054990585</v>
+        <v>0.02559475217996412</v>
       </c>
       <c r="J7" t="n">
-        <v>0.7170912174623177</v>
+        <v>0.01706316811997605</v>
       </c>
     </row>
     <row r="8">
@@ -676,28 +676,28 @@
         <v>0</v>
       </c>
       <c r="C8" t="n">
-        <v>0.1599042420244978</v>
+        <v>0.02180821962234357</v>
       </c>
       <c r="D8" t="n">
-        <v>0.4873425835973605</v>
+        <v>0.04361643924468724</v>
       </c>
       <c r="E8" t="n">
-        <v>0.3889554917817489</v>
+        <v>0.02180821962234376</v>
       </c>
       <c r="F8" t="n">
-        <v>0.02478433142834971</v>
+        <v>0.06542465886703092</v>
       </c>
       <c r="G8" t="n">
-        <v>0.4355673159495371</v>
+        <v>0.04361643924468742</v>
       </c>
       <c r="H8" t="n">
-        <v>0.488464116688771</v>
+        <v>0.06542465886703108</v>
       </c>
       <c r="I8" t="n">
-        <v>0.3713553935524667</v>
+        <v>0.130849317734062</v>
       </c>
       <c r="J8" t="n">
-        <v>0.465296978401158</v>
+        <v>0.08723287848937468</v>
       </c>
     </row>
     <row r="9">
@@ -710,28 +710,28 @@
         <v>0</v>
       </c>
       <c r="C9" t="n">
-        <v>0.08492603540588145</v>
+        <v>0.007324199000941048</v>
       </c>
       <c r="D9" t="n">
-        <v>0.3934881152184632</v>
+        <v>0.01464839800188193</v>
       </c>
       <c r="E9" t="n">
-        <v>0.5176193094290396</v>
+        <v>0.007324199000940878</v>
       </c>
       <c r="F9" t="n">
-        <v>0.2483276680368304</v>
+        <v>0.02197259700282288</v>
       </c>
       <c r="G9" t="n">
-        <v>0.424949187557659</v>
+        <v>0.01464839800188183</v>
       </c>
       <c r="H9" t="n">
-        <v>0.4050866709826863</v>
+        <v>0.02197259700282271</v>
       </c>
       <c r="I9" t="n">
-        <v>0.5556072474601554</v>
+        <v>0.04394519400564559</v>
       </c>
       <c r="J9" t="n">
-        <v>0.6450257546195728</v>
+        <v>0.02929679600376376</v>
       </c>
     </row>
     <row r="10">
@@ -744,28 +744,28 @@
         <v>0</v>
       </c>
       <c r="C10" t="n">
-        <v>0.08626174301803335</v>
+        <v>0.01388057970233389</v>
       </c>
       <c r="D10" t="n">
-        <v>0.1749260040156308</v>
+        <v>0.02776115940466778</v>
       </c>
       <c r="E10" t="n">
-        <v>0.3388081320031547</v>
+        <v>0.01388057970233388</v>
       </c>
       <c r="F10" t="n">
-        <v>0.226570013319835</v>
+        <v>0.04164173910700156</v>
       </c>
       <c r="G10" t="n">
-        <v>0.1818961809789129</v>
+        <v>0.02776115940466768</v>
       </c>
       <c r="H10" t="n">
-        <v>0.2363870609818441</v>
+        <v>0.04164173910700146</v>
       </c>
       <c r="I10" t="n">
-        <v>0.2887379663633927</v>
+        <v>0.08328347821400302</v>
       </c>
       <c r="J10" t="n">
-        <v>0.4544728450955593</v>
+        <v>0.05552231880933533</v>
       </c>
     </row>
     <row r="11">
@@ -778,28 +778,28 @@
         <v>0</v>
       </c>
       <c r="C11" t="n">
-        <v>0.4791548834846637</v>
+        <v>0.05155846797659717</v>
       </c>
       <c r="D11" t="n">
-        <v>0.4206831656561428</v>
+        <v>0.1031169359531942</v>
       </c>
       <c r="E11" t="n">
-        <v>0.7576469300251578</v>
+        <v>0.05155846797659698</v>
       </c>
       <c r="F11" t="n">
-        <v>0.4420403105303157</v>
+        <v>0.1546754039297912</v>
       </c>
       <c r="G11" t="n">
-        <v>0.297409475050477</v>
+        <v>0.1031169359531941</v>
       </c>
       <c r="H11" t="n">
-        <v>0.706963690814697</v>
+        <v>0.1546754039297911</v>
       </c>
       <c r="I11" t="n">
-        <v>0.707870236715073</v>
+        <v>0.3093508078595822</v>
       </c>
       <c r="J11" t="n">
-        <v>0.7555817318408117</v>
+        <v>0.2062338719063881</v>
       </c>
     </row>
     <row r="12">
@@ -812,28 +812,28 @@
         <v>0</v>
       </c>
       <c r="C12" t="n">
-        <v>0.08626174301803725</v>
+        <v>0.01162168521397276</v>
       </c>
       <c r="D12" t="n">
-        <v>0.1749260040152817</v>
+        <v>0.02324337042794564</v>
       </c>
       <c r="E12" t="n">
-        <v>0.3388081320003999</v>
+        <v>0.01162168521397285</v>
       </c>
       <c r="F12" t="n">
-        <v>0.2265700133196986</v>
+        <v>0.03486505564191849</v>
       </c>
       <c r="G12" t="n">
-        <v>0.1818961809786989</v>
+        <v>0.02324337042794579</v>
       </c>
       <c r="H12" t="n">
-        <v>0.2363870609818421</v>
+        <v>0.03486505564191864</v>
       </c>
       <c r="I12" t="n">
-        <v>0.2887379663598593</v>
+        <v>0.06973011128383713</v>
       </c>
       <c r="J12" t="n">
-        <v>0.4544728450898249</v>
+        <v>0.0464867408558915</v>
       </c>
     </row>
     <row r="13">
@@ -846,28 +846,28 @@
         <v>0</v>
       </c>
       <c r="C13" t="n">
-        <v>0.2451171397259831</v>
+        <v>0.02431058797811773</v>
       </c>
       <c r="D13" t="n">
-        <v>0.1578389977439907</v>
+        <v>0.0486211759562355</v>
       </c>
       <c r="E13" t="n">
-        <v>0.08137120693072791</v>
+        <v>0.02431058797811765</v>
       </c>
       <c r="F13" t="n">
-        <v>0.05675540978200554</v>
+        <v>0.07293176393435323</v>
       </c>
       <c r="G13" t="n">
-        <v>0.2387375396095963</v>
+        <v>0.04862117595623548</v>
       </c>
       <c r="H13" t="n">
-        <v>0.1135927951325067</v>
+        <v>0.07293176393435313</v>
       </c>
       <c r="I13" t="n">
-        <v>0.08218402802539798</v>
+        <v>0.1458635278687063</v>
       </c>
       <c r="J13" t="n">
-        <v>0.482127729462026</v>
+        <v>0.09724235191247088</v>
       </c>
     </row>
     <row r="14">
@@ -880,28 +880,28 @@
         <v>0</v>
       </c>
       <c r="C14" t="n">
-        <v>0.05032188755287357</v>
+        <v>0.002435470696372353</v>
       </c>
       <c r="D14" t="n">
-        <v>0.0651512596997411</v>
+        <v>0.004870941392744757</v>
       </c>
       <c r="E14" t="n">
-        <v>0.1173638886129968</v>
+        <v>0.002435470696372404</v>
       </c>
       <c r="F14" t="n">
-        <v>0.046915137466223</v>
+        <v>0.007306412089117144</v>
       </c>
       <c r="G14" t="n">
-        <v>0.0291964564058739</v>
+        <v>0.004870941392744792</v>
       </c>
       <c r="H14" t="n">
-        <v>0.1303829890717259</v>
+        <v>0.007306412089117261</v>
       </c>
       <c r="I14" t="n">
-        <v>0.2525115858017104</v>
+        <v>0.0146128241782344</v>
       </c>
       <c r="J14" t="n">
-        <v>0.2946200681905465</v>
+        <v>0.009741882785489648</v>
       </c>
     </row>
     <row r="15">
@@ -914,28 +914,28 @@
         <v>0</v>
       </c>
       <c r="C15" t="n">
-        <v>0.05239320222149003</v>
+        <v>0.003769656843364089</v>
       </c>
       <c r="D15" t="n">
-        <v>0.2230234971813184</v>
+        <v>0.007539313686728323</v>
       </c>
       <c r="E15" t="n">
-        <v>0.5213189820481547</v>
+        <v>0.003769656843364123</v>
       </c>
       <c r="F15" t="n">
-        <v>0.1850352178249533</v>
+        <v>0.01130897053009239</v>
       </c>
       <c r="G15" t="n">
-        <v>0.4313621678109487</v>
+        <v>0.007539313686728309</v>
       </c>
       <c r="H15" t="n">
-        <v>0.4084918931616273</v>
+        <v>0.01130897053009243</v>
       </c>
       <c r="I15" t="n">
-        <v>0.6309536095993336</v>
+        <v>0.02261794106018482</v>
       </c>
       <c r="J15" t="n">
-        <v>0.6956985276791432</v>
+        <v>0.01507862737345652</v>
       </c>
     </row>
     <row r="16">
@@ -948,28 +948,28 @@
         <v>0</v>
       </c>
       <c r="C16" t="n">
-        <v>0.01683044603760741</v>
+        <v>0.02030988836669417</v>
       </c>
       <c r="D16" t="n">
-        <v>0.0947639091223135</v>
+        <v>0.04061977673338836</v>
       </c>
       <c r="E16" t="n">
-        <v>0.18897143636735</v>
+        <v>0.0203098883666941</v>
       </c>
       <c r="F16" t="n">
-        <v>0.09549135763695685</v>
+        <v>0.06092966510008245</v>
       </c>
       <c r="G16" t="n">
-        <v>0.07333903633776524</v>
+        <v>0.04061977673338828</v>
       </c>
       <c r="H16" t="n">
-        <v>0.1337539785750796</v>
+        <v>0.06092966510008238</v>
       </c>
       <c r="I16" t="n">
-        <v>0.3298667033007553</v>
+        <v>0.1218593302001648</v>
       </c>
       <c r="J16" t="n">
-        <v>0.4409583259818232</v>
+        <v>0.08123955346677655</v>
       </c>
     </row>
     <row r="17">
@@ -982,28 +982,28 @@
         <v>0</v>
       </c>
       <c r="C17" t="n">
-        <v>0.03903815153014736</v>
+        <v>0.0006876968899117854</v>
       </c>
       <c r="D17" t="n">
-        <v>0.2689956312071948</v>
+        <v>0.001375393779823474</v>
       </c>
       <c r="E17" t="n">
-        <v>0.618848773385095</v>
+        <v>0.0006876968899117142</v>
       </c>
       <c r="F17" t="n">
-        <v>0.1281531536638903</v>
+        <v>0.002063090669735162</v>
       </c>
       <c r="G17" t="n">
-        <v>0.08640740296582554</v>
+        <v>0.001375393779823377</v>
       </c>
       <c r="H17" t="n">
-        <v>0.4188096615522368</v>
+        <v>0.002063090669735091</v>
       </c>
       <c r="I17" t="n">
-        <v>0.6319524848028147</v>
+        <v>0.00412618133947028</v>
       </c>
       <c r="J17" t="n">
-        <v>0.6872975258654004</v>
+        <v>0.002750787559646904</v>
       </c>
     </row>
     <row r="18">
@@ -1016,28 +1016,28 @@
         <v>0</v>
       </c>
       <c r="C18" t="n">
-        <v>0.01670039006815244</v>
+        <v>0.007303228522353748</v>
       </c>
       <c r="D18" t="n">
-        <v>0.03865679330888044</v>
+        <v>0.01460645704470749</v>
       </c>
       <c r="E18" t="n">
-        <v>0.0541591935160668</v>
+        <v>0.007303228522353616</v>
       </c>
       <c r="F18" t="n">
-        <v>0.0218554289296818</v>
+        <v>0.02190968556706121</v>
       </c>
       <c r="G18" t="n">
-        <v>0.3253323198980465</v>
+        <v>0.01460645704470741</v>
       </c>
       <c r="H18" t="n">
-        <v>0.2381118491482621</v>
+        <v>0.02190968556706121</v>
       </c>
       <c r="I18" t="n">
-        <v>0.1026639973125949</v>
+        <v>0.04381937113412236</v>
       </c>
       <c r="J18" t="n">
-        <v>0.1957006154131989</v>
+        <v>0.02921291408941489</v>
       </c>
     </row>
     <row r="19">
@@ -1050,28 +1050,28 @@
         <v>0</v>
       </c>
       <c r="C19" t="n">
-        <v>0.006934670056590476</v>
+        <v>0.001905751655668409</v>
       </c>
       <c r="D19" t="n">
-        <v>0.04121661327330469</v>
+        <v>0.003811503311336879</v>
       </c>
       <c r="E19" t="n">
-        <v>0.2471172541182301</v>
+        <v>0.00190575165566834</v>
       </c>
       <c r="F19" t="n">
-        <v>0.1998593668199364</v>
+        <v>0.005717254967005185</v>
       </c>
       <c r="G19" t="n">
-        <v>0.05993853628225231</v>
+        <v>0.003811503311336732</v>
       </c>
       <c r="H19" t="n">
-        <v>0.07007428236768669</v>
+        <v>0.005717254967005099</v>
       </c>
       <c r="I19" t="n">
-        <v>0.4088213153973929</v>
+        <v>0.01143450993401026</v>
       </c>
       <c r="J19" t="n">
-        <v>0.4947271340347213</v>
+        <v>0.007623006622673508</v>
       </c>
     </row>
     <row r="20">
@@ -1084,28 +1084,28 @@
         <v>0</v>
       </c>
       <c r="C20" t="n">
-        <v>0.03518414443353168</v>
+        <v>0.01241575855806621</v>
       </c>
       <c r="D20" t="n">
-        <v>0.06795099009753248</v>
+        <v>0.02483151711613242</v>
       </c>
       <c r="E20" t="n">
-        <v>0.2663788873957219</v>
+        <v>0.01241575855806614</v>
       </c>
       <c r="F20" t="n">
-        <v>0.07380679970766253</v>
+        <v>0.03724727567419856</v>
       </c>
       <c r="G20" t="n">
-        <v>0.1024729724739653</v>
+        <v>0.02483151711613235</v>
       </c>
       <c r="H20" t="n">
-        <v>0.1568833585515501</v>
+        <v>0.03724727567419848</v>
       </c>
       <c r="I20" t="n">
-        <v>0.3097723229462173</v>
+        <v>0.07449455134839704</v>
       </c>
       <c r="J20" t="n">
-        <v>0.6340282210191579</v>
+        <v>0.0496630342322647</v>
       </c>
     </row>
     <row r="21">
@@ -1118,28 +1118,28 @@
         <v>0</v>
       </c>
       <c r="C21" t="n">
-        <v>0.006934670056601891</v>
+        <v>0.01924993406000224</v>
       </c>
       <c r="D21" t="n">
-        <v>0.04121661327253895</v>
+        <v>0.03849986812000462</v>
       </c>
       <c r="E21" t="n">
-        <v>0.2471172541224445</v>
+        <v>0.0192499340600023</v>
       </c>
       <c r="F21" t="n">
-        <v>0.1998593668216571</v>
+        <v>0.05774980218000685</v>
       </c>
       <c r="G21" t="n">
-        <v>0.05993853628351726</v>
+        <v>0.03849986812000461</v>
       </c>
       <c r="H21" t="n">
-        <v>0.07007428236768413</v>
+        <v>0.05774980218000691</v>
       </c>
       <c r="I21" t="n">
-        <v>0.408821315403501</v>
+        <v>0.1154996043600138</v>
       </c>
       <c r="J21" t="n">
-        <v>0.4947271340443923</v>
+        <v>0.07699973624000915</v>
       </c>
     </row>
     <row r="22">
@@ -1152,28 +1152,28 @@
         <v>0</v>
       </c>
       <c r="C22" t="n">
-        <v>0.05239320222149237</v>
+        <v>0.004960025362020695</v>
       </c>
       <c r="D22" t="n">
-        <v>0.2230234971806837</v>
+        <v>0.009920050724041308</v>
       </c>
       <c r="E22" t="n">
-        <v>0.5213189820286916</v>
+        <v>0.004960025362020604</v>
       </c>
       <c r="F22" t="n">
-        <v>0.1850352178193981</v>
+        <v>0.01488007608606189</v>
       </c>
       <c r="G22" t="n">
-        <v>0.431362167807376</v>
+        <v>0.009920050724041217</v>
       </c>
       <c r="H22" t="n">
-        <v>0.4084918931615183</v>
+        <v>0.0148800760860618</v>
       </c>
       <c r="I22" t="n">
-        <v>0.6309536095760827</v>
+        <v>0.02976015217212371</v>
       </c>
       <c r="J22" t="n">
-        <v>0.6956985276804495</v>
+        <v>0.01984010144808251</v>
       </c>
     </row>
     <row r="23">
@@ -1186,28 +1186,28 @@
         <v>0</v>
       </c>
       <c r="C23" t="n">
-        <v>0.0168304460376051</v>
+        <v>0.005069500098151526</v>
       </c>
       <c r="D23" t="n">
-        <v>0.09476390912399844</v>
+        <v>0.01013900019630322</v>
       </c>
       <c r="E23" t="n">
-        <v>0.1889714363827729</v>
+        <v>0.005069500098151639</v>
       </c>
       <c r="F23" t="n">
-        <v>0.095491357646297</v>
+        <v>0.01520850029445485</v>
       </c>
       <c r="G23" t="n">
-        <v>0.07333903633900707</v>
+        <v>0.0101390001963033</v>
       </c>
       <c r="H23" t="n">
-        <v>0.1337539785751161</v>
+        <v>0.01520850029445494</v>
       </c>
       <c r="I23" t="n">
-        <v>0.329866703317071</v>
+        <v>0.03041700058890979</v>
       </c>
       <c r="J23" t="n">
-        <v>0.4409583260078945</v>
+        <v>0.02027800039260657</v>
       </c>
     </row>
     <row r="24">
@@ -1220,28 +1220,28 @@
         <v>0</v>
       </c>
       <c r="C24" t="n">
-        <v>0.0390381515301588</v>
+        <v>0.01483409318935364</v>
       </c>
       <c r="D24" t="n">
-        <v>0.2689956312087648</v>
+        <v>0.02966818637870732</v>
       </c>
       <c r="E24" t="n">
-        <v>0.6188487733927751</v>
+        <v>0.01483409318935368</v>
       </c>
       <c r="F24" t="n">
-        <v>0.1281531536709437</v>
+        <v>0.04450227956806091</v>
       </c>
       <c r="G24" t="n">
-        <v>0.08640740296744961</v>
+        <v>0.02966818637870721</v>
       </c>
       <c r="H24" t="n">
-        <v>0.4188096615522802</v>
+        <v>0.04450227956806089</v>
       </c>
       <c r="I24" t="n">
-        <v>0.6319524848132515</v>
+        <v>0.08900455913612178</v>
       </c>
       <c r="J24" t="n">
-        <v>0.6872975258811979</v>
+        <v>0.05933637275741453</v>
       </c>
     </row>
     <row r="25">
@@ -1254,28 +1254,28 @@
         <v>0</v>
       </c>
       <c r="C25" t="n">
-        <v>0.05032188755287368</v>
+        <v>0.00692772811322721</v>
       </c>
       <c r="D25" t="n">
-        <v>0.06515125969977451</v>
+        <v>0.0138554562264545</v>
       </c>
       <c r="E25" t="n">
-        <v>0.1173638886139998</v>
+        <v>0.006927728113227288</v>
       </c>
       <c r="F25" t="n">
-        <v>0.04691513746689529</v>
+        <v>0.02078318433968171</v>
       </c>
       <c r="G25" t="n">
-        <v>0.02919645640632213</v>
+        <v>0.0138554562264545</v>
       </c>
       <c r="H25" t="n">
-        <v>0.1303829890717177</v>
+        <v>0.02078318433968179</v>
       </c>
       <c r="I25" t="n">
-        <v>0.2525115858011427</v>
+        <v>0.0415663686793635</v>
       </c>
       <c r="J25" t="n">
-        <v>0.2946200681915583</v>
+        <v>0.027710912452909</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
some updates the past few weeks yeah
</commit_message>
<xml_diff>
--- a/06_distance_LitoLi_intercage_litype4_CONTCAR_positive_0.xlsx
+++ b/06_distance_LitoLi_intercage_litype4_CONTCAR_positive_0.xlsx
@@ -472,28 +472,28 @@
         <v>0</v>
       </c>
       <c r="C2" t="n">
-        <v>0.002767164346438711</v>
+        <v>0.1221089063380579</v>
       </c>
       <c r="D2" t="n">
-        <v>0.005534328692877489</v>
+        <v>0.05667183572656422</v>
       </c>
       <c r="E2" t="n">
-        <v>0.002767164346438755</v>
+        <v>0.3211595485804488</v>
       </c>
       <c r="F2" t="n">
-        <v>0.008301493039316252</v>
+        <v>0.2193388286095951</v>
       </c>
       <c r="G2" t="n">
-        <v>0.005534328692877542</v>
+        <v>0.1415814790529661</v>
       </c>
       <c r="H2" t="n">
-        <v>0.008301493039316252</v>
+        <v>0.1910585783618671</v>
       </c>
       <c r="I2" t="n">
-        <v>0.0166029860786326</v>
+        <v>0.02490447911794885</v>
       </c>
       <c r="J2" t="n">
-        <v>0.0110686573857551</v>
+        <v>0.08715245548174068</v>
       </c>
     </row>
     <row r="3">
@@ -506,28 +506,28 @@
         <v>0</v>
       </c>
       <c r="C3" t="n">
-        <v>0.001396708916112762</v>
+        <v>0.0521406020907713</v>
       </c>
       <c r="D3" t="n">
-        <v>0.0027934178322257</v>
+        <v>0.3532589433180323</v>
       </c>
       <c r="E3" t="n">
-        <v>0.001396708916112888</v>
+        <v>0.6710434694221715</v>
       </c>
       <c r="F3" t="n">
-        <v>0.004190126748338587</v>
+        <v>0.5877335378547766</v>
       </c>
       <c r="G3" t="n">
-        <v>0.002793417832225825</v>
+        <v>0.5157913150014871</v>
       </c>
       <c r="H3" t="n">
-        <v>0.004190126748338714</v>
+        <v>0.5570805888616498</v>
       </c>
       <c r="I3" t="n">
-        <v>0.008380253496677301</v>
+        <v>0.01257038024501589</v>
       </c>
       <c r="J3" t="n">
-        <v>0.005586835664451475</v>
+        <v>0.3815832249538377</v>
       </c>
     </row>
     <row r="4">
@@ -540,28 +540,28 @@
         <v>0</v>
       </c>
       <c r="C4" t="n">
-        <v>0.01709710209335594</v>
+        <v>0.06061850427318792</v>
       </c>
       <c r="D4" t="n">
-        <v>0.03419420418671198</v>
+        <v>0.05272820037210534</v>
       </c>
       <c r="E4" t="n">
-        <v>0.01709710209335608</v>
+        <v>0.2161304025387943</v>
       </c>
       <c r="F4" t="n">
-        <v>0.05129130628006797</v>
+        <v>0.3166335343525982</v>
       </c>
       <c r="G4" t="n">
-        <v>0.0341942041867121</v>
+        <v>0.2149017587941981</v>
       </c>
       <c r="H4" t="n">
-        <v>0.05129130628006809</v>
+        <v>0.2141689417392107</v>
       </c>
       <c r="I4" t="n">
-        <v>0.1025826125601361</v>
+        <v>0.1538739188402041</v>
       </c>
       <c r="J4" t="n">
-        <v>0.06838840837342415</v>
+        <v>0.06661064523310527</v>
       </c>
     </row>
     <row r="5">
@@ -574,28 +574,28 @@
         <v>0</v>
       </c>
       <c r="C5" t="n">
-        <v>0.008776272009646518</v>
+        <v>0.05236527680284045</v>
       </c>
       <c r="D5" t="n">
-        <v>0.0175525440192929</v>
+        <v>0.2727019875170374</v>
       </c>
       <c r="E5" t="n">
-        <v>0.008776272009646428</v>
+        <v>0.4466589320811828</v>
       </c>
       <c r="F5" t="n">
-        <v>0.02632881602893943</v>
+        <v>0.5029279674534891</v>
       </c>
       <c r="G5" t="n">
-        <v>0.01755254401929289</v>
+        <v>0.5941951608508814</v>
       </c>
       <c r="H5" t="n">
-        <v>0.02632881602893932</v>
+        <v>0.5421197261852483</v>
       </c>
       <c r="I5" t="n">
-        <v>0.05265763205787874</v>
+        <v>0.07898644808681816</v>
       </c>
       <c r="J5" t="n">
-        <v>0.03510508803858584</v>
+        <v>0.2940878029595256</v>
       </c>
     </row>
     <row r="6">
@@ -608,28 +608,28 @@
         <v>0</v>
       </c>
       <c r="C6" t="n">
-        <v>0.0045608954098372</v>
+        <v>0.2504702820923962</v>
       </c>
       <c r="D6" t="n">
-        <v>0.009121790819674305</v>
+        <v>0.1931191904018958</v>
       </c>
       <c r="E6" t="n">
-        <v>0.004560895409837224</v>
+        <v>0.2968538858314453</v>
       </c>
       <c r="F6" t="n">
-        <v>0.0136826862295115</v>
+        <v>0.2530993598845906</v>
       </c>
       <c r="G6" t="n">
-        <v>0.009121790819674274</v>
+        <v>0.1317844090981011</v>
       </c>
       <c r="H6" t="n">
-        <v>0.01368268622951148</v>
+        <v>0.1761312533493202</v>
       </c>
       <c r="I6" t="n">
-        <v>0.027365372459023</v>
+        <v>0.04104805868853451</v>
       </c>
       <c r="J6" t="n">
-        <v>0.0182435816393487</v>
+        <v>0.2044926820048217</v>
       </c>
     </row>
     <row r="7">
@@ -642,28 +642,28 @@
         <v>0</v>
       </c>
       <c r="C7" t="n">
-        <v>0.004265792029994007</v>
+        <v>0.1523271065783985</v>
       </c>
       <c r="D7" t="n">
-        <v>0.008531584059987994</v>
+        <v>0.4728680878765464</v>
       </c>
       <c r="E7" t="n">
-        <v>0.004265792029993986</v>
+        <v>0.3895165000223245</v>
       </c>
       <c r="F7" t="n">
-        <v>0.01279737608998207</v>
+        <v>0.3220876412301786</v>
       </c>
       <c r="G7" t="n">
-        <v>0.008531584059988061</v>
+        <v>0.3638931718703192</v>
       </c>
       <c r="H7" t="n">
-        <v>0.01279737608998205</v>
+        <v>0.3436376859969555</v>
       </c>
       <c r="I7" t="n">
-        <v>0.02559475217996412</v>
+        <v>0.03839212826994619</v>
       </c>
       <c r="J7" t="n">
-        <v>0.01706316811997605</v>
+        <v>0.4091561293709164</v>
       </c>
     </row>
     <row r="8">
@@ -676,28 +676,28 @@
         <v>0</v>
       </c>
       <c r="C8" t="n">
-        <v>0.02180821962234357</v>
+        <v>0.1562042908344657</v>
       </c>
       <c r="D8" t="n">
-        <v>0.04361643924468724</v>
+        <v>0.1836026026006673</v>
       </c>
       <c r="E8" t="n">
-        <v>0.02180821962234376</v>
+        <v>0.4867276688979716</v>
       </c>
       <c r="F8" t="n">
-        <v>0.06542465886703092</v>
+        <v>0.3767857758787648</v>
       </c>
       <c r="G8" t="n">
-        <v>0.04361643924468742</v>
+        <v>0.3020545768112137</v>
       </c>
       <c r="H8" t="n">
-        <v>0.06542465886703108</v>
+        <v>0.3582755530718278</v>
       </c>
       <c r="I8" t="n">
-        <v>0.130849317734062</v>
+        <v>0.196273976601093</v>
       </c>
       <c r="J8" t="n">
-        <v>0.08723287848937468</v>
+        <v>0.1801164855031319</v>
       </c>
     </row>
     <row r="9">
@@ -710,28 +710,28 @@
         <v>0</v>
       </c>
       <c r="C9" t="n">
-        <v>0.007324199000941048</v>
+        <v>0.110999018595311</v>
       </c>
       <c r="D9" t="n">
-        <v>0.01464839800188193</v>
+        <v>0.05750540359501723</v>
       </c>
       <c r="E9" t="n">
-        <v>0.007324199000940878</v>
+        <v>0.2678921817048892</v>
       </c>
       <c r="F9" t="n">
-        <v>0.02197259700282288</v>
+        <v>0.2878747055431122</v>
       </c>
       <c r="G9" t="n">
-        <v>0.01464839800188183</v>
+        <v>0.2543634632311458</v>
       </c>
       <c r="H9" t="n">
-        <v>0.02197259700282271</v>
+        <v>0.300310610456655</v>
       </c>
       <c r="I9" t="n">
-        <v>0.04394519400564559</v>
+        <v>0.06591779100846847</v>
       </c>
       <c r="J9" t="n">
-        <v>0.02929679600376376</v>
+        <v>0.06450445058865004</v>
       </c>
     </row>
     <row r="10">
@@ -744,28 +744,28 @@
         <v>0</v>
       </c>
       <c r="C10" t="n">
-        <v>0.01388057970233389</v>
+        <v>0.3555411626094466</v>
       </c>
       <c r="D10" t="n">
-        <v>0.02776115940466778</v>
+        <v>0.3890580211478373</v>
       </c>
       <c r="E10" t="n">
-        <v>0.01388057970233388</v>
+        <v>0.1976322408940027</v>
       </c>
       <c r="F10" t="n">
-        <v>0.04164173910700156</v>
+        <v>0.06426727500536926</v>
       </c>
       <c r="G10" t="n">
-        <v>0.02776115940466768</v>
+        <v>0.1315463511749019</v>
       </c>
       <c r="H10" t="n">
-        <v>0.04164173910700146</v>
+        <v>0.07470209583380527</v>
       </c>
       <c r="I10" t="n">
-        <v>0.08328347821400302</v>
+        <v>0.1249252173210046</v>
       </c>
       <c r="J10" t="n">
-        <v>0.05552231880933533</v>
+        <v>0.2191580708406993</v>
       </c>
     </row>
     <row r="11">
@@ -778,28 +778,28 @@
         <v>0</v>
       </c>
       <c r="C11" t="n">
-        <v>0.05155846797659717</v>
+        <v>0.2916408856922709</v>
       </c>
       <c r="D11" t="n">
-        <v>0.1031169359531942</v>
+        <v>0.2949881489384521</v>
       </c>
       <c r="E11" t="n">
-        <v>0.05155846797659698</v>
+        <v>0.3486749359084462</v>
       </c>
       <c r="F11" t="n">
-        <v>0.1546754039297912</v>
+        <v>0.3783540089594553</v>
       </c>
       <c r="G11" t="n">
-        <v>0.1031169359531941</v>
+        <v>0.1657765384589845</v>
       </c>
       <c r="H11" t="n">
-        <v>0.1546754039297911</v>
+        <v>0.3133925709457292</v>
       </c>
       <c r="I11" t="n">
-        <v>0.3093508078595822</v>
+        <v>0.4640262117893734</v>
       </c>
       <c r="J11" t="n">
-        <v>0.2062338719063881</v>
+        <v>0.2180542334657396</v>
       </c>
     </row>
     <row r="12">
@@ -812,28 +812,28 @@
         <v>0</v>
       </c>
       <c r="C12" t="n">
-        <v>0.01162168521397276</v>
+        <v>0.05694529914590994</v>
       </c>
       <c r="D12" t="n">
-        <v>0.02324337042794564</v>
+        <v>0.1261039145409353</v>
       </c>
       <c r="E12" t="n">
-        <v>0.01162168521397285</v>
+        <v>0.3993798401154126</v>
       </c>
       <c r="F12" t="n">
-        <v>0.03486505564191849</v>
+        <v>0.2232839199634121</v>
       </c>
       <c r="G12" t="n">
-        <v>0.02324337042794579</v>
+        <v>0.209771203020897</v>
       </c>
       <c r="H12" t="n">
-        <v>0.03486505564191864</v>
+        <v>0.2251856991234587</v>
       </c>
       <c r="I12" t="n">
-        <v>0.06973011128383713</v>
+        <v>0.1045951669257556</v>
       </c>
       <c r="J12" t="n">
-        <v>0.0464867408558915</v>
+        <v>0.1073151451188274</v>
       </c>
     </row>
     <row r="13">
@@ -846,28 +846,28 @@
         <v>0</v>
       </c>
       <c r="C13" t="n">
-        <v>0.02431058797811773</v>
+        <v>0.02999454772084903</v>
       </c>
       <c r="D13" t="n">
-        <v>0.0486211759562355</v>
+        <v>0.1655854160283751</v>
       </c>
       <c r="E13" t="n">
-        <v>0.02431058797811765</v>
+        <v>0.2850121201910394</v>
       </c>
       <c r="F13" t="n">
-        <v>0.07293176393435323</v>
+        <v>0.2024456846945018</v>
       </c>
       <c r="G13" t="n">
-        <v>0.04862117595623548</v>
+        <v>0.1743710317806629</v>
       </c>
       <c r="H13" t="n">
-        <v>0.07293176393435313</v>
+        <v>0.1475431396275167</v>
       </c>
       <c r="I13" t="n">
-        <v>0.1458635278687063</v>
+        <v>0.2187952918030596</v>
       </c>
       <c r="J13" t="n">
-        <v>0.09724235191247088</v>
+        <v>0.1387895025337578</v>
       </c>
     </row>
     <row r="14">
@@ -880,28 +880,28 @@
         <v>0</v>
       </c>
       <c r="C14" t="n">
-        <v>0.002435470696372353</v>
+        <v>0.3346598016955187</v>
       </c>
       <c r="D14" t="n">
-        <v>0.004870941392744757</v>
+        <v>0.4173411504166115</v>
       </c>
       <c r="E14" t="n">
-        <v>0.002435470696372404</v>
+        <v>0.5155403708011996</v>
       </c>
       <c r="F14" t="n">
-        <v>0.007306412089117144</v>
+        <v>0.5767381663888015</v>
       </c>
       <c r="G14" t="n">
-        <v>0.004870941392744792</v>
+        <v>0.4962656372070536</v>
       </c>
       <c r="H14" t="n">
-        <v>0.007306412089117261</v>
+        <v>0.4904983353506448</v>
       </c>
       <c r="I14" t="n">
-        <v>0.0146128241782344</v>
+        <v>0.02191923626735155</v>
       </c>
       <c r="J14" t="n">
-        <v>0.009741882785489648</v>
+        <v>0.3340372793447789</v>
       </c>
     </row>
     <row r="15">
@@ -914,28 +914,28 @@
         <v>0</v>
       </c>
       <c r="C15" t="n">
-        <v>0.003769656843364089</v>
+        <v>0.3101110215720707</v>
       </c>
       <c r="D15" t="n">
-        <v>0.007539313686728323</v>
+        <v>0.2919151534546408</v>
       </c>
       <c r="E15" t="n">
-        <v>0.003769656843364123</v>
+        <v>0.4034107821138355</v>
       </c>
       <c r="F15" t="n">
-        <v>0.01130897053009239</v>
+        <v>0.300149119480917</v>
       </c>
       <c r="G15" t="n">
-        <v>0.007539313686728309</v>
+        <v>0.2029541637292397</v>
       </c>
       <c r="H15" t="n">
-        <v>0.01130897053009243</v>
+        <v>0.3171388721944635</v>
       </c>
       <c r="I15" t="n">
-        <v>0.02261794106018482</v>
+        <v>0.03392691159027722</v>
       </c>
       <c r="J15" t="n">
-        <v>0.01507862737345652</v>
+        <v>0.302848360067093</v>
       </c>
     </row>
     <row r="16">
@@ -948,28 +948,28 @@
         <v>0</v>
       </c>
       <c r="C16" t="n">
-        <v>0.02030988836669417</v>
+        <v>0.1430306054787642</v>
       </c>
       <c r="D16" t="n">
-        <v>0.04061977673338836</v>
+        <v>0.2708874560637792</v>
       </c>
       <c r="E16" t="n">
-        <v>0.0203098883666941</v>
+        <v>0.6177783880851135</v>
       </c>
       <c r="F16" t="n">
-        <v>0.06092966510008245</v>
+        <v>0.4660143435166007</v>
       </c>
       <c r="G16" t="n">
-        <v>0.04061977673338828</v>
+        <v>0.3049137444030126</v>
       </c>
       <c r="H16" t="n">
-        <v>0.06092966510008238</v>
+        <v>0.333223401824376</v>
       </c>
       <c r="I16" t="n">
-        <v>0.1218593302001648</v>
+        <v>0.1827889953002473</v>
       </c>
       <c r="J16" t="n">
-        <v>0.08123955346677655</v>
+        <v>0.1243117779858766</v>
       </c>
     </row>
     <row r="17">
@@ -982,28 +982,28 @@
         <v>0</v>
       </c>
       <c r="C17" t="n">
-        <v>0.0006876968899117854</v>
+        <v>0.2986124684659847</v>
       </c>
       <c r="D17" t="n">
-        <v>0.001375393779823474</v>
+        <v>0.2915008351073351</v>
       </c>
       <c r="E17" t="n">
-        <v>0.0006876968899117142</v>
+        <v>0.6204184786470422</v>
       </c>
       <c r="F17" t="n">
-        <v>0.002063090669735162</v>
+        <v>0.6651269427960155</v>
       </c>
       <c r="G17" t="n">
-        <v>0.001375393779823377</v>
+        <v>0.533512656677863</v>
       </c>
       <c r="H17" t="n">
-        <v>0.002063090669735091</v>
+        <v>0.5879749931444529</v>
       </c>
       <c r="I17" t="n">
-        <v>0.00412618133947028</v>
+        <v>0.006189272009205444</v>
       </c>
       <c r="J17" t="n">
-        <v>0.002750787559646904</v>
+        <v>0.2911961486013736</v>
       </c>
     </row>
     <row r="18">
@@ -1016,28 +1016,28 @@
         <v>0</v>
       </c>
       <c r="C18" t="n">
-        <v>0.007303228522353748</v>
+        <v>0.3049196220952002</v>
       </c>
       <c r="D18" t="n">
-        <v>0.01460645704470749</v>
+        <v>0.5867896226282683</v>
       </c>
       <c r="E18" t="n">
-        <v>0.007303228522353616</v>
+        <v>0.6646755233824322</v>
       </c>
       <c r="F18" t="n">
-        <v>0.02190968556706121</v>
+        <v>0.6527563095190463</v>
       </c>
       <c r="G18" t="n">
-        <v>0.01460645704470741</v>
+        <v>0.5702477869729837</v>
       </c>
       <c r="H18" t="n">
-        <v>0.02190968556706121</v>
+        <v>0.488614381560924</v>
       </c>
       <c r="I18" t="n">
-        <v>0.04381937113412236</v>
+        <v>0.06572905670118356</v>
       </c>
       <c r="J18" t="n">
-        <v>0.02921291408941489</v>
+        <v>0.4061570297407783</v>
       </c>
     </row>
     <row r="19">
@@ -1050,28 +1050,28 @@
         <v>0</v>
       </c>
       <c r="C19" t="n">
-        <v>0.001905751655668409</v>
+        <v>0.2730433218116961</v>
       </c>
       <c r="D19" t="n">
-        <v>0.003811503311336879</v>
+        <v>0.3692725404981654</v>
       </c>
       <c r="E19" t="n">
-        <v>0.00190575165566834</v>
+        <v>0.3643682281803224</v>
       </c>
       <c r="F19" t="n">
-        <v>0.005717254967005185</v>
+        <v>0.5218528830593737</v>
       </c>
       <c r="G19" t="n">
-        <v>0.003811503311336732</v>
+        <v>0.4739422182336951</v>
       </c>
       <c r="H19" t="n">
-        <v>0.005717254967005099</v>
+        <v>0.5146898778335515</v>
       </c>
       <c r="I19" t="n">
-        <v>0.01143450993401026</v>
+        <v>0.01715176490101544</v>
       </c>
       <c r="J19" t="n">
-        <v>0.007623006622673508</v>
+        <v>0.3073278356572086</v>
       </c>
     </row>
     <row r="20">
@@ -1084,28 +1084,28 @@
         <v>0</v>
       </c>
       <c r="C20" t="n">
-        <v>0.01241575855806621</v>
+        <v>0.2025036683650922</v>
       </c>
       <c r="D20" t="n">
-        <v>0.02483151711613242</v>
+        <v>0.214333569215466</v>
       </c>
       <c r="E20" t="n">
-        <v>0.01241575855806614</v>
+        <v>0.2973776141360639</v>
       </c>
       <c r="F20" t="n">
-        <v>0.03724727567419856</v>
+        <v>0.2403703570472182</v>
       </c>
       <c r="G20" t="n">
-        <v>0.02483151711613235</v>
+        <v>0.2619818583713167</v>
       </c>
       <c r="H20" t="n">
-        <v>0.03724727567419848</v>
+        <v>0.2251790251343379</v>
       </c>
       <c r="I20" t="n">
-        <v>0.07449455134839704</v>
+        <v>0.1117418270225956</v>
       </c>
       <c r="J20" t="n">
-        <v>0.0496630342322647</v>
+        <v>0.1780892119188407</v>
       </c>
     </row>
     <row r="21">
@@ -1118,28 +1118,28 @@
         <v>0</v>
       </c>
       <c r="C21" t="n">
-        <v>0.01924993406000224</v>
+        <v>0.2295611529714554</v>
       </c>
       <c r="D21" t="n">
-        <v>0.03849986812000462</v>
+        <v>0.4221420735844187</v>
       </c>
       <c r="E21" t="n">
-        <v>0.0192499340600023</v>
+        <v>0.6061319196989261</v>
       </c>
       <c r="F21" t="n">
-        <v>0.05774980218000685</v>
+        <v>0.5387636084583555</v>
       </c>
       <c r="G21" t="n">
-        <v>0.03849986812000461</v>
+        <v>0.5472891506367564</v>
       </c>
       <c r="H21" t="n">
-        <v>0.05774980218000691</v>
+        <v>0.5075474056752981</v>
       </c>
       <c r="I21" t="n">
-        <v>0.1154996043600138</v>
+        <v>0.1732494065400206</v>
       </c>
       <c r="J21" t="n">
-        <v>0.07699973624000915</v>
+        <v>0.3944532975639055</v>
       </c>
     </row>
     <row r="22">
@@ -1152,28 +1152,28 @@
         <v>0</v>
       </c>
       <c r="C22" t="n">
-        <v>0.004960025362020695</v>
+        <v>0.2720063863017567</v>
       </c>
       <c r="D22" t="n">
-        <v>0.009920050724041308</v>
+        <v>0.1567008811481451</v>
       </c>
       <c r="E22" t="n">
-        <v>0.004960025362020604</v>
+        <v>0.427342897950528</v>
       </c>
       <c r="F22" t="n">
-        <v>0.01488007608606189</v>
+        <v>0.2864239863294233</v>
       </c>
       <c r="G22" t="n">
-        <v>0.009920050724041217</v>
+        <v>0.1418987071935987</v>
       </c>
       <c r="H22" t="n">
-        <v>0.0148800760860618</v>
+        <v>0.2245200748804823</v>
       </c>
       <c r="I22" t="n">
-        <v>0.02976015217212371</v>
+        <v>0.0446402282581856</v>
       </c>
       <c r="J22" t="n">
-        <v>0.01984010144808251</v>
+        <v>0.1133086345571219</v>
       </c>
     </row>
     <row r="23">
@@ -1186,28 +1186,28 @@
         <v>0</v>
       </c>
       <c r="C23" t="n">
-        <v>0.005069500098151526</v>
+        <v>0.150641714080226</v>
       </c>
       <c r="D23" t="n">
-        <v>0.01013900019630322</v>
+        <v>0.3833547985668339</v>
       </c>
       <c r="E23" t="n">
-        <v>0.005069500098151639</v>
+        <v>0.6234743306603664</v>
       </c>
       <c r="F23" t="n">
-        <v>0.01520850029445485</v>
+        <v>0.6558536924011198</v>
       </c>
       <c r="G23" t="n">
-        <v>0.0101390001963033</v>
+        <v>0.5177023903577762</v>
       </c>
       <c r="H23" t="n">
-        <v>0.01520850029445494</v>
+        <v>0.5753083671493943</v>
       </c>
       <c r="I23" t="n">
-        <v>0.03041700058890979</v>
+        <v>0.04562550088336464</v>
       </c>
       <c r="J23" t="n">
-        <v>0.02027800039260657</v>
+        <v>0.3367232312751348</v>
       </c>
     </row>
     <row r="24">
@@ -1220,28 +1220,28 @@
         <v>0</v>
       </c>
       <c r="C24" t="n">
-        <v>0.01483409318935364</v>
+        <v>0.1540082716866467</v>
       </c>
       <c r="D24" t="n">
-        <v>0.02966818637870732</v>
+        <v>0.3427044964394886</v>
       </c>
       <c r="E24" t="n">
-        <v>0.01483409318935368</v>
+        <v>0.5456800975731519</v>
       </c>
       <c r="F24" t="n">
-        <v>0.04450227956806091</v>
+        <v>0.515025256662373</v>
       </c>
       <c r="G24" t="n">
-        <v>0.02966818637870721</v>
+        <v>0.4655227203131477</v>
       </c>
       <c r="H24" t="n">
-        <v>0.04450227956806089</v>
+        <v>0.4914646086840925</v>
       </c>
       <c r="I24" t="n">
-        <v>0.08900455913612178</v>
+        <v>0.1335068387041827</v>
       </c>
       <c r="J24" t="n">
-        <v>0.05933637275741453</v>
+        <v>0.2863582778424957</v>
       </c>
     </row>
     <row r="25">
@@ -1254,28 +1254,28 @@
         <v>0</v>
       </c>
       <c r="C25" t="n">
-        <v>0.00692772811322721</v>
+        <v>0.3323439558694475</v>
       </c>
       <c r="D25" t="n">
-        <v>0.0138554562264545</v>
+        <v>0.4323057290783849</v>
       </c>
       <c r="E25" t="n">
-        <v>0.006927728113227288</v>
+        <v>0.2861082711539883</v>
       </c>
       <c r="F25" t="n">
-        <v>0.02078318433968171</v>
+        <v>0.475748258487646</v>
       </c>
       <c r="G25" t="n">
-        <v>0.0138554562264545</v>
+        <v>0.4547685833270968</v>
       </c>
       <c r="H25" t="n">
-        <v>0.02078318433968179</v>
+        <v>0.4255959456203076</v>
       </c>
       <c r="I25" t="n">
-        <v>0.0415663686793635</v>
+        <v>0.0623495530190452</v>
       </c>
       <c r="J25" t="n">
-        <v>0.027710912452909</v>
+        <v>0.391163424321444</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
before splitting branc for correcting idx_atom, idx_cage, et
</commit_message>
<xml_diff>
--- a/06_distance_LitoLi_intercage_litype4_CONTCAR_positive_0.xlsx
+++ b/06_distance_LitoLi_intercage_litype4_CONTCAR_positive_0.xlsx
@@ -472,28 +472,28 @@
         <v>0</v>
       </c>
       <c r="C2" t="n">
-        <v>0.009229980275325693</v>
+        <v>0.01505956653180308</v>
       </c>
       <c r="D2" t="n">
-        <v>0.03600095518069574</v>
+        <v>0.006655508476755214</v>
       </c>
       <c r="E2" t="n">
-        <v>0.02569982264102135</v>
+        <v>0.005540725634798621</v>
       </c>
       <c r="F2" t="n">
-        <v>0.03474998320128772</v>
+        <v>0.007213228778664049</v>
       </c>
       <c r="G2" t="n">
-        <v>0.01633355832796288</v>
+        <v>0.001725375263283578</v>
       </c>
       <c r="H2" t="n">
-        <v>0.0787804830960598</v>
+        <v>0.003267032367985395</v>
       </c>
       <c r="I2" t="n">
-        <v>0.1349222142836668</v>
+        <v>0.004873094951432177</v>
       </c>
       <c r="J2" t="n">
-        <v>0.1343771662872143</v>
+        <v>0.005543367401200143</v>
       </c>
     </row>
     <row r="3">
@@ -506,28 +506,28 @@
         <v>0</v>
       </c>
       <c r="C3" t="n">
-        <v>0.04159337537377752</v>
+        <v>0.005153323810632863</v>
       </c>
       <c r="D3" t="n">
-        <v>0.02876419353689283</v>
+        <v>0.002532400444471825</v>
       </c>
       <c r="E3" t="n">
-        <v>0.04990421121988182</v>
+        <v>0.01896935445428094</v>
       </c>
       <c r="F3" t="n">
-        <v>0.1256220491567051</v>
+        <v>0.02136475261612573</v>
       </c>
       <c r="G3" t="n">
-        <v>0.01733397816548228</v>
+        <v>0.02242601898829309</v>
       </c>
       <c r="H3" t="n">
-        <v>0.04680464288363901</v>
+        <v>0.02293233898858835</v>
       </c>
       <c r="I3" t="n">
-        <v>0.1009166324744821</v>
+        <v>0.02297239994926484</v>
       </c>
       <c r="J3" t="n">
-        <v>0.09781484356609602</v>
+        <v>0.02164933638070174</v>
       </c>
     </row>
     <row r="4">
@@ -540,28 +540,28 @@
         <v>0</v>
       </c>
       <c r="C4" t="n">
-        <v>0.06060794748010435</v>
+        <v>0.02214439202959719</v>
       </c>
       <c r="D4" t="n">
-        <v>0.0654949309841054</v>
+        <v>0.005460109069908542</v>
       </c>
       <c r="E4" t="n">
-        <v>0.08043038688192994</v>
+        <v>0.004941565667234192</v>
       </c>
       <c r="F4" t="n">
-        <v>0.07113324619383148</v>
+        <v>0.01005120654486235</v>
       </c>
       <c r="G4" t="n">
-        <v>0.05552520742294337</v>
+        <v>0.01195009060986179</v>
       </c>
       <c r="H4" t="n">
-        <v>0.04752361243457141</v>
+        <v>0.008691884552270997</v>
       </c>
       <c r="I4" t="n">
-        <v>0.0380646476117051</v>
+        <v>0.006551750336519168</v>
       </c>
       <c r="J4" t="n">
-        <v>0.0401749378436134</v>
+        <v>0.006156427107321682</v>
       </c>
     </row>
     <row r="5">
@@ -574,28 +574,28 @@
         <v>0</v>
       </c>
       <c r="C5" t="n">
-        <v>0.2388920226700659</v>
+        <v>0.02478238888413976</v>
       </c>
       <c r="D5" t="n">
-        <v>0.3449651413483223</v>
+        <v>0.01241360749151886</v>
       </c>
       <c r="E5" t="n">
-        <v>0.1557112440619544</v>
+        <v>0.02188726207441022</v>
       </c>
       <c r="F5" t="n">
-        <v>0.3544478544575035</v>
+        <v>0.04933775663039652</v>
       </c>
       <c r="G5" t="n">
-        <v>0.03569200019750918</v>
+        <v>0.06799622630634698</v>
       </c>
       <c r="H5" t="n">
-        <v>0.2583012759509716</v>
+        <v>0.05864019243215166</v>
       </c>
       <c r="I5" t="n">
-        <v>0.2806283459563491</v>
+        <v>0.05532956737522657</v>
       </c>
       <c r="J5" t="n">
-        <v>0.2778147261469694</v>
+        <v>0.05438525409536313</v>
       </c>
     </row>
     <row r="6">
@@ -608,28 +608,28 @@
         <v>0</v>
       </c>
       <c r="C6" t="n">
-        <v>0.01547271504665782</v>
+        <v>0.01225545359969111</v>
       </c>
       <c r="D6" t="n">
-        <v>0.02333571139067789</v>
+        <v>0.007528418663735556</v>
       </c>
       <c r="E6" t="n">
-        <v>0.06115211549899024</v>
+        <v>0.01178810099147961</v>
       </c>
       <c r="F6" t="n">
-        <v>0.02343980067754829</v>
+        <v>0.01778772713318658</v>
       </c>
       <c r="G6" t="n">
-        <v>0.004723511702597657</v>
+        <v>0.0123460304811311</v>
       </c>
       <c r="H6" t="n">
-        <v>0.1030858758244267</v>
+        <v>0.01219587910722672</v>
       </c>
       <c r="I6" t="n">
-        <v>0.08597101952257624</v>
+        <v>0.01502502810293069</v>
       </c>
       <c r="J6" t="n">
-        <v>0.08640605398571215</v>
+        <v>0.01585371562957804</v>
       </c>
     </row>
     <row r="7">
@@ -642,28 +642,28 @@
         <v>0</v>
       </c>
       <c r="C7" t="n">
-        <v>0.04783471490349667</v>
+        <v>0.01849929498210313</v>
       </c>
       <c r="D7" t="n">
-        <v>0.09385088349180051</v>
+        <v>0.01322577549246233</v>
       </c>
       <c r="E7" t="n">
-        <v>0.2000776668237274</v>
+        <v>0.07298940583576695</v>
       </c>
       <c r="F7" t="n">
-        <v>0.2110373055521778</v>
+        <v>0.1670235332444248</v>
       </c>
       <c r="G7" t="n">
-        <v>0.3205147472087029</v>
+        <v>0.1710294211295618</v>
       </c>
       <c r="H7" t="n">
-        <v>0.2176914476016003</v>
+        <v>0.1678085710264902</v>
       </c>
       <c r="I7" t="n">
-        <v>0.2943024188444289</v>
+        <v>0.1678532705046736</v>
       </c>
       <c r="J7" t="n">
-        <v>0.2881374741343665</v>
+        <v>0.1685859543563264</v>
       </c>
     </row>
     <row r="8">
@@ -676,28 +676,28 @@
         <v>0</v>
       </c>
       <c r="C8" t="n">
-        <v>0.03870996942716692</v>
+        <v>0.03788725546164584</v>
       </c>
       <c r="D8" t="n">
-        <v>0.01598631529384971</v>
+        <v>0.01373343574963775</v>
       </c>
       <c r="E8" t="n">
-        <v>0.09492728371057693</v>
+        <v>0.006331012163750279</v>
       </c>
       <c r="F8" t="n">
-        <v>0.01631084413557889</v>
+        <v>0.008487582253415215</v>
       </c>
       <c r="G8" t="n">
-        <v>0.03644230188441801</v>
+        <v>0.01959160869151961</v>
       </c>
       <c r="H8" t="n">
-        <v>0.04708320720266743</v>
+        <v>0.01932112183336477</v>
       </c>
       <c r="I8" t="n">
-        <v>0.03130555305050291</v>
+        <v>0.01982698470353078</v>
       </c>
       <c r="J8" t="n">
-        <v>0.02932499536177223</v>
+        <v>0.0200955266932417</v>
       </c>
     </row>
     <row r="9">
@@ -710,28 +710,28 @@
         <v>0</v>
       </c>
       <c r="C9" t="n">
-        <v>0.008548623480558171</v>
+        <v>0.1123295359585581</v>
       </c>
       <c r="D9" t="n">
-        <v>0.07332877051785659</v>
+        <v>0.0676806987907083</v>
       </c>
       <c r="E9" t="n">
-        <v>0.04485728187242173</v>
+        <v>0.007374149378138057</v>
       </c>
       <c r="F9" t="n">
-        <v>0.02837283934261666</v>
+        <v>0.0109178601972343</v>
       </c>
       <c r="G9" t="n">
-        <v>0.002848747451039677</v>
+        <v>0.01988642725312672</v>
       </c>
       <c r="H9" t="n">
-        <v>0.02420991302672338</v>
+        <v>0.01666852797736826</v>
       </c>
       <c r="I9" t="n">
-        <v>0.06741426909562258</v>
+        <v>0.01478910331523276</v>
       </c>
       <c r="J9" t="n">
-        <v>0.05916688484088726</v>
+        <v>0.01401878313223462</v>
       </c>
     </row>
     <row r="10">
@@ -744,28 +744,28 @@
         <v>0</v>
       </c>
       <c r="C10" t="n">
-        <v>0.1973384747909222</v>
+        <v>0.01416259051265287</v>
       </c>
       <c r="D10" t="n">
-        <v>0.3221357366069392</v>
+        <v>0.007724610685865659</v>
       </c>
       <c r="E10" t="n">
-        <v>0.1598637898880165</v>
+        <v>0.01058566032828587</v>
       </c>
       <c r="F10" t="n">
-        <v>0.2458907290611204</v>
+        <v>0.05452214575040266</v>
       </c>
       <c r="G10" t="n">
-        <v>0.2185108390223551</v>
+        <v>0.1046205590897365</v>
       </c>
       <c r="H10" t="n">
-        <v>0.1921401796678525</v>
+        <v>0.07858290965217565</v>
       </c>
       <c r="I10" t="n">
-        <v>0.2256697321943906</v>
+        <v>0.06484484377742704</v>
       </c>
       <c r="J10" t="n">
-        <v>0.2254340686946437</v>
+        <v>0.06359626769401394</v>
       </c>
     </row>
     <row r="11">
@@ -778,28 +778,28 @@
         <v>0</v>
       </c>
       <c r="C11" t="n">
-        <v>0.0135492990457726</v>
+        <v>0.01329807462044543</v>
       </c>
       <c r="D11" t="n">
-        <v>0.01254494550753137</v>
+        <v>0.005004379119870251</v>
       </c>
       <c r="E11" t="n">
-        <v>0.02104666541725369</v>
+        <v>0.07624946880774604</v>
       </c>
       <c r="F11" t="n">
-        <v>0.02805619630928546</v>
+        <v>0.104755935394209</v>
       </c>
       <c r="G11" t="n">
-        <v>0.01226487367870991</v>
+        <v>0.2476169872448132</v>
       </c>
       <c r="H11" t="n">
-        <v>0.0257726202032245</v>
+        <v>0.2390190803712388</v>
       </c>
       <c r="I11" t="n">
-        <v>0.03980632106947694</v>
+        <v>0.2144986871836984</v>
       </c>
       <c r="J11" t="n">
-        <v>0.03879153172150298</v>
+        <v>0.1846342691116284</v>
       </c>
     </row>
     <row r="12">
@@ -812,28 +812,28 @@
         <v>0</v>
       </c>
       <c r="C12" t="n">
-        <v>0.01283802627653877</v>
+        <v>0.03334622209700434</v>
       </c>
       <c r="D12" t="n">
-        <v>0.0118259816930165</v>
+        <v>0.01901765371181997</v>
       </c>
       <c r="E12" t="n">
-        <v>0.05322450173540556</v>
+        <v>0.009477492555591794</v>
       </c>
       <c r="F12" t="n">
-        <v>0.05139192891505295</v>
+        <v>0.01014181161619434</v>
       </c>
       <c r="G12" t="n">
-        <v>0.01607543136632422</v>
+        <v>0.02414134848830692</v>
       </c>
       <c r="H12" t="n">
-        <v>0.02380811695476279</v>
+        <v>0.01939142667867981</v>
       </c>
       <c r="I12" t="n">
-        <v>0.0391410251514517</v>
+        <v>0.01441576670015966</v>
       </c>
       <c r="J12" t="n">
-        <v>0.04080826915455237</v>
+        <v>0.011137756693358</v>
       </c>
     </row>
     <row r="13">
@@ -846,28 +846,28 @@
         <v>0</v>
       </c>
       <c r="C13" t="n">
-        <v>0.05555104622928686</v>
+        <v>0.1117658987003902</v>
       </c>
       <c r="D13" t="n">
-        <v>0.02117055239794534</v>
+        <v>0.02473565285159378</v>
       </c>
       <c r="E13" t="n">
-        <v>0.04568860347762968</v>
+        <v>0.004680921824752451</v>
       </c>
       <c r="F13" t="n">
-        <v>0.02997478329808327</v>
+        <v>0.002389937772437547</v>
       </c>
       <c r="G13" t="n">
-        <v>0.0445915270215865</v>
+        <v>0.003233807175893693</v>
       </c>
       <c r="H13" t="n">
-        <v>0.0694322283418423</v>
+        <v>0.004372816710611909</v>
       </c>
       <c r="I13" t="n">
-        <v>0.2104623949302019</v>
+        <v>0.004150334492120327</v>
       </c>
       <c r="J13" t="n">
-        <v>0.2111121224869872</v>
+        <v>0.003541739253984812</v>
       </c>
     </row>
     <row r="14">
@@ -880,28 +880,28 @@
         <v>0</v>
       </c>
       <c r="C14" t="n">
-        <v>0.1867742949220563</v>
+        <v>0.00557407816565549</v>
       </c>
       <c r="D14" t="n">
-        <v>0.2639310422605077</v>
+        <v>0.005761385161390136</v>
       </c>
       <c r="E14" t="n">
-        <v>0.02148143201956177</v>
+        <v>0.0153631644502335</v>
       </c>
       <c r="F14" t="n">
-        <v>0.04378207898139046</v>
+        <v>0.02389595381142297</v>
       </c>
       <c r="G14" t="n">
-        <v>0.04231049568488439</v>
+        <v>0.03890247095227292</v>
       </c>
       <c r="H14" t="n">
-        <v>0.1517024743337536</v>
+        <v>0.03329701233998805</v>
       </c>
       <c r="I14" t="n">
-        <v>0.2538055351997506</v>
+        <v>0.02999697908923857</v>
       </c>
       <c r="J14" t="n">
-        <v>0.249887336326143</v>
+        <v>0.02938606452994983</v>
       </c>
     </row>
     <row r="15">
@@ -914,28 +914,28 @@
         <v>0</v>
       </c>
       <c r="C15" t="n">
-        <v>0.0359645582951808</v>
+        <v>0.05631423013119357</v>
       </c>
       <c r="D15" t="n">
-        <v>0.01418936692607485</v>
+        <v>0.008783896415226145</v>
       </c>
       <c r="E15" t="n">
-        <v>0.1155632418420952</v>
+        <v>0.01506786180845653</v>
       </c>
       <c r="F15" t="n">
-        <v>0.05038332865767792</v>
+        <v>0.04009776004427446</v>
       </c>
       <c r="G15" t="n">
-        <v>0.03724511586314418</v>
+        <v>0.09514459113556638</v>
       </c>
       <c r="H15" t="n">
-        <v>0.02595072320741547</v>
+        <v>0.0882561972245625</v>
       </c>
       <c r="I15" t="n">
-        <v>0.07483208636263065</v>
+        <v>0.07813207808085504</v>
       </c>
       <c r="J15" t="n">
-        <v>0.07383937447771009</v>
+        <v>0.07144255182842971</v>
       </c>
     </row>
     <row r="16">
@@ -948,28 +948,28 @@
         <v>0</v>
       </c>
       <c r="C16" t="n">
-        <v>0.008344471413082708</v>
+        <v>0.01708215049612046</v>
       </c>
       <c r="D16" t="n">
-        <v>0.01753089943381613</v>
+        <v>0.005815399506113059</v>
       </c>
       <c r="E16" t="n">
-        <v>0.06068823426139276</v>
+        <v>0.0139330278687159</v>
       </c>
       <c r="F16" t="n">
-        <v>0.04765019125892777</v>
+        <v>0.02608608166600109</v>
       </c>
       <c r="G16" t="n">
-        <v>0.006931583166542633</v>
+        <v>0.05782788157352283</v>
       </c>
       <c r="H16" t="n">
-        <v>0.003546201472919268</v>
+        <v>0.05426876869872535</v>
       </c>
       <c r="I16" t="n">
-        <v>0.01712561834538347</v>
+        <v>0.04752278674955638</v>
       </c>
       <c r="J16" t="n">
-        <v>0.01749428484097852</v>
+        <v>0.04155012568209795</v>
       </c>
     </row>
     <row r="17">
@@ -982,28 +982,28 @@
         <v>0</v>
       </c>
       <c r="C17" t="n">
-        <v>0.03000953019237014</v>
+        <v>0.02759569020580487</v>
       </c>
       <c r="D17" t="n">
-        <v>0.01393591067543611</v>
+        <v>0.0234465870331998</v>
       </c>
       <c r="E17" t="n">
-        <v>0.006232853279635736</v>
+        <v>0.01826120080147743</v>
       </c>
       <c r="F17" t="n">
-        <v>0.01461079187055543</v>
+        <v>0.0263438837543765</v>
       </c>
       <c r="G17" t="n">
-        <v>0.01618386661302909</v>
+        <v>0.03433625620756707</v>
       </c>
       <c r="H17" t="n">
-        <v>0.03178318710423887</v>
+        <v>0.03339916868694447</v>
       </c>
       <c r="I17" t="n">
-        <v>0.2172655812619183</v>
+        <v>0.03560687525791097</v>
       </c>
       <c r="J17" t="n">
-        <v>0.2185639075890345</v>
+        <v>0.03668905160837609</v>
       </c>
     </row>
     <row r="18">
@@ -1016,28 +1016,28 @@
         <v>0</v>
       </c>
       <c r="C18" t="n">
-        <v>0.03963667264756913</v>
+        <v>0.01078756207624328</v>
       </c>
       <c r="D18" t="n">
-        <v>0.02954523548327666</v>
+        <v>0.004843972373330935</v>
       </c>
       <c r="E18" t="n">
-        <v>0.03522075633657182</v>
+        <v>0.01321990397504768</v>
       </c>
       <c r="F18" t="n">
-        <v>0.04623241152209717</v>
+        <v>0.01463252975579887</v>
       </c>
       <c r="G18" t="n">
-        <v>0.03034845898509458</v>
+        <v>0.02420365451375114</v>
       </c>
       <c r="H18" t="n">
-        <v>0.01545261478355936</v>
+        <v>0.02253426938717498</v>
       </c>
       <c r="I18" t="n">
-        <v>0.1032962331116222</v>
+        <v>0.01987314163372758</v>
       </c>
       <c r="J18" t="n">
-        <v>0.09859438629379404</v>
+        <v>0.01790559106518226</v>
       </c>
     </row>
     <row r="19">
@@ -1050,28 +1050,28 @@
         <v>0</v>
       </c>
       <c r="C19" t="n">
-        <v>0.2334950258285565</v>
+        <v>0.02374721349482608</v>
       </c>
       <c r="D19" t="n">
-        <v>0.3272753176054904</v>
+        <v>0.01404411453077162</v>
       </c>
       <c r="E19" t="n">
-        <v>0.03360518299552406</v>
+        <v>0.03128805468497187</v>
       </c>
       <c r="F19" t="n">
-        <v>0.1762859277065432</v>
+        <v>0.06132706466938106</v>
       </c>
       <c r="G19" t="n">
-        <v>0.03731019834610321</v>
+        <v>0.06965073995152941</v>
       </c>
       <c r="H19" t="n">
-        <v>0.219472258435859</v>
+        <v>0.06642945090004945</v>
       </c>
       <c r="I19" t="n">
-        <v>0.2566777819543605</v>
+        <v>0.06590343760311514</v>
       </c>
       <c r="J19" t="n">
-        <v>0.2498303591084045</v>
+        <v>0.06600208614093368</v>
       </c>
     </row>
     <row r="20">
@@ -1084,28 +1084,28 @@
         <v>0</v>
       </c>
       <c r="C20" t="n">
-        <v>0.02328907026715912</v>
+        <v>0.02438488942127046</v>
       </c>
       <c r="D20" t="n">
-        <v>0.1098702450632054</v>
+        <v>0.01992866845875498</v>
       </c>
       <c r="E20" t="n">
-        <v>0.08676040013295627</v>
+        <v>0.005983947965266301</v>
       </c>
       <c r="F20" t="n">
-        <v>0.1111154980636015</v>
+        <v>0.01235512592693053</v>
       </c>
       <c r="G20" t="n">
-        <v>0.0970647412961456</v>
+        <v>0.01796615462683873</v>
       </c>
       <c r="H20" t="n">
-        <v>0.03625749264929534</v>
+        <v>0.01534681365895521</v>
       </c>
       <c r="I20" t="n">
-        <v>0.069906326621959</v>
+        <v>0.0137781517248359</v>
       </c>
       <c r="J20" t="n">
-        <v>0.06051036490861251</v>
+        <v>0.01349799605080589</v>
       </c>
     </row>
     <row r="21">
@@ -1118,28 +1118,28 @@
         <v>0</v>
       </c>
       <c r="C21" t="n">
-        <v>0.01551338454943551</v>
+        <v>0.01482942871766625</v>
       </c>
       <c r="D21" t="n">
-        <v>0.003679429686654466</v>
+        <v>0.0008207716307635523</v>
       </c>
       <c r="E21" t="n">
-        <v>0.03573620585603225</v>
+        <v>0.005576165001748302</v>
       </c>
       <c r="F21" t="n">
-        <v>0.03277426548588706</v>
+        <v>0.008366368446422854</v>
       </c>
       <c r="G21" t="n">
-        <v>0.008611080043741138</v>
+        <v>0.01510725090272155</v>
       </c>
       <c r="H21" t="n">
-        <v>0.0290629215243348</v>
+        <v>0.01479747058377699</v>
       </c>
       <c r="I21" t="n">
-        <v>0.05372950006153228</v>
+        <v>0.01463687721552361</v>
       </c>
       <c r="J21" t="n">
-        <v>0.05240002224026542</v>
+        <v>0.01308988911319072</v>
       </c>
     </row>
     <row r="22">
@@ -1152,28 +1152,28 @@
         <v>0</v>
       </c>
       <c r="C22" t="n">
-        <v>0.01519069988155782</v>
+        <v>0.009406257684587953</v>
       </c>
       <c r="D22" t="n">
-        <v>0.02110445133949816</v>
+        <v>0.007409922220980187</v>
       </c>
       <c r="E22" t="n">
-        <v>0.01830948396462509</v>
+        <v>0.0192433685650105</v>
       </c>
       <c r="F22" t="n">
-        <v>0.03131985169208547</v>
+        <v>0.02486720818491086</v>
       </c>
       <c r="G22" t="n">
-        <v>0.01576702855036166</v>
+        <v>0.01227372563748423</v>
       </c>
       <c r="H22" t="n">
-        <v>0.04116158803187588</v>
+        <v>0.01453715696600799</v>
       </c>
       <c r="I22" t="n">
-        <v>0.05262910858284138</v>
+        <v>0.01650015248389613</v>
       </c>
       <c r="J22" t="n">
-        <v>0.05101085894490835</v>
+        <v>0.01801680501480611</v>
       </c>
     </row>
     <row r="23">
@@ -1186,28 +1186,28 @@
         <v>0</v>
       </c>
       <c r="C23" t="n">
-        <v>0.07602474611603224</v>
+        <v>0.00913018812540917</v>
       </c>
       <c r="D23" t="n">
-        <v>0.2641315349866581</v>
+        <v>0.009012332788868973</v>
       </c>
       <c r="E23" t="n">
-        <v>0.1721077058799069</v>
+        <v>0.003548907939936044</v>
       </c>
       <c r="F23" t="n">
-        <v>0.2265861832522582</v>
+        <v>0.02669626646638929</v>
       </c>
       <c r="G23" t="n">
-        <v>0.1909465210625249</v>
+        <v>0.03848255718178404</v>
       </c>
       <c r="H23" t="n">
-        <v>0.1688656071759696</v>
+        <v>0.03068922808573128</v>
       </c>
       <c r="I23" t="n">
-        <v>0.1968912926294323</v>
+        <v>0.0257591808355581</v>
       </c>
       <c r="J23" t="n">
-        <v>0.1957629956119313</v>
+        <v>0.02534229307507111</v>
       </c>
     </row>
     <row r="24">
@@ -1220,28 +1220,28 @@
         <v>0</v>
       </c>
       <c r="C24" t="n">
-        <v>0.02252543342521952</v>
+        <v>0.09853351062668951</v>
       </c>
       <c r="D24" t="n">
-        <v>0.02955418649832032</v>
+        <v>0.0884925849001703</v>
       </c>
       <c r="E24" t="n">
-        <v>0.04892426665763893</v>
+        <v>0.02507017144110394</v>
       </c>
       <c r="F24" t="n">
-        <v>0.03569415144708253</v>
+        <v>0.03647207647875175</v>
       </c>
       <c r="G24" t="n">
-        <v>0.04095012340119936</v>
+        <v>0.03947215462152264</v>
       </c>
       <c r="H24" t="n">
-        <v>0.01870218608989238</v>
+        <v>0.03499527543275315</v>
       </c>
       <c r="I24" t="n">
-        <v>0.02257057865852698</v>
+        <v>0.03262744497867312</v>
       </c>
       <c r="J24" t="n">
-        <v>0.02144953427950506</v>
+        <v>0.03223493684906135</v>
       </c>
     </row>
     <row r="25">
@@ -1254,28 +1254,28 @@
         <v>0</v>
       </c>
       <c r="C25" t="n">
-        <v>0.01800224432130374</v>
+        <v>0.03095691844094778</v>
       </c>
       <c r="D25" t="n">
-        <v>0.03287955233062323</v>
+        <v>0.02116590734507894</v>
       </c>
       <c r="E25" t="n">
-        <v>0.1321517625099056</v>
+        <v>0.01133997796818447</v>
       </c>
       <c r="F25" t="n">
-        <v>0.1357106931256823</v>
+        <v>0.03204610427004737</v>
       </c>
       <c r="G25" t="n">
-        <v>0.03228483157925079</v>
+        <v>0.02223979218100981</v>
       </c>
       <c r="H25" t="n">
-        <v>0.02667239512645876</v>
+        <v>0.02246502598274192</v>
       </c>
       <c r="I25" t="n">
-        <v>0.02795611071338481</v>
+        <v>0.02538221008646805</v>
       </c>
       <c r="J25" t="n">
-        <v>0.02440440450779298</v>
+        <v>0.02772911555182953</v>
       </c>
     </row>
   </sheetData>

</xml_diff>